<commit_message>
encryption in transit started
</commit_message>
<xml_diff>
--- a/frontend/public/BULK_DP_UPLOAD_FORMAT.xlsx
+++ b/frontend/public/BULK_DP_UPLOAD_FORMAT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Akzo(CB-Intrade)\CB-Intrade-Akzo-\frontend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CB-Intrade(Vesuvius)\CB-Intrade-Vesuvius\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -93,9 +93,6 @@
     <t>RelationType</t>
   </si>
   <si>
-    <t xml:space="preserve">Akshay Kumar </t>
-  </si>
-  <si>
     <t>Sonam Kumar</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>OFFICER</t>
   </si>
   <si>
-    <t xml:space="preserve">kumar.akki@gmail.com </t>
-  </si>
-  <si>
     <t>A45PR6530M</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
   </si>
   <si>
     <t>SUB-INSIDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kumar.sonam@gmail.com </t>
   </si>
   <si>
     <t>A654PR6730W</t>
@@ -149,6 +140,15 @@
   <si>
     <t>90002005/01</t>
   </si>
+  <si>
+    <t>kumar.akki@gmail.com</t>
+  </si>
+  <si>
+    <t>kumar.sonam@gmail.com</t>
+  </si>
+  <si>
+    <t>Akshay Kumar</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -199,15 +199,10 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF1155CC"/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -248,8 +243,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -284,7 +280,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -300,7 +295,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -316,8 +310,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,8 +533,8 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -558,11 +555,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>40</v>
+      <c r="F1" s="31" t="s">
+        <v>37</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>41</v>
+      <c r="G1" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
@@ -622,7 +619,7 @@
         <v>23</v>
       </c>
       <c r="AA1" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AD1" s="11"/>
     </row>
@@ -631,40 +628,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="34">
+      <c r="F2" s="32">
         <v>90002005</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="19"/>
       <c r="K2" s="17"/>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="21" t="s">
         <v>29</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="O2" s="17">
         <v>400</v>
       </c>
-      <c r="P2" s="21"/>
+      <c r="P2" s="20"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
       <c r="S2" s="18"/>
@@ -672,62 +669,62 @@
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="X2" s="19"/>
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" s="10"/>
+    </row>
+    <row r="3" spans="1:30" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="10"/>
-    </row>
-    <row r="3" spans="1:30" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
-        <v>2</v>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="35" t="s">
+        <v>41</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>25</v>
+      <c r="M3" s="27" t="s">
+        <v>32</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26" t="s">
+      <c r="N3" s="28"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35" t="s">
-        <v>42</v>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26" t="s">
+        <v>30</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="28" t="s">
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA3" s="32"/>
+      <c r="AA3" s="30"/>
       <c r="AD3" s="10"/>
     </row>
     <row r="4" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>